<commit_message>
Integração Tela/Lógica Parte 1
Os botões de geração de gráfico e leitura/carregamento da planilha funcionam.
</commit_message>
<xml_diff>
--- a/DOW/tabelastest/TabelasEx.xlsx
+++ b/DOW/tabelastest/TabelasEx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\ProjetoDOW-main\DOW\tabelastest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF96811E-C70F-4DA4-84DF-6943A35726A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC98B91-686C-40FC-870A-017E2F2C56F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="615" windowWidth="21840" windowHeight="13140" xr2:uid="{A535ECC4-06C6-4676-8CE5-90DAE0234A8C}"/>
+    <workbookView xWindow="3615" yWindow="2295" windowWidth="16200" windowHeight="9360" xr2:uid="{A535ECC4-06C6-4676-8CE5-90DAE0234A8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -503,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD53D9B6-8549-4B30-B785-6BD17C328FBB}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,7 @@
         <v>39</v>
       </c>
       <c r="G3" s="9">
-        <f>F3-F2</f>
+        <f t="shared" ref="G3:G8" si="0">F3-F2</f>
         <v>21</v>
       </c>
     </row>
@@ -600,7 +600,7 @@
         <v>64</v>
       </c>
       <c r="G4" s="9">
-        <f>F4-F3</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -621,7 +621,7 @@
         <v>93</v>
       </c>
       <c r="G5" s="9">
-        <f>F5-F4</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
@@ -643,7 +643,7 @@
         <v>115</v>
       </c>
       <c r="G6" s="9">
-        <f>F6-F5</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
@@ -664,7 +664,7 @@
         <v>132</v>
       </c>
       <c r="G7" s="9">
-        <f>F7-F6</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
@@ -686,7 +686,7 @@
         <v>140</v>
       </c>
       <c r="G8" s="9">
-        <f>F8-F7</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -720,12 +720,6 @@
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <f>SUM(B2:B9)</f>
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Selecionar planilhas e salvar gráfico
Agora é possível selecionar entre as planilhas do arquivo e salvar o gráfico gerado pela planilha escolhida no excel.
</commit_message>
<xml_diff>
--- a/DOW/tabelastest/TabelasEx.xlsx
+++ b/DOW/tabelastest/TabelasEx.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\ProjetoDOW-main\DOW\tabelastest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC98B91-686C-40FC-870A-017E2F2C56F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423791E3-27EC-4CDE-81A8-9905EE271166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="2295" windowWidth="16200" windowHeight="9360" xr2:uid="{A535ECC4-06C6-4676-8CE5-90DAE0234A8C}"/>
+    <workbookView xWindow="3615" yWindow="2295" windowWidth="16200" windowHeight="9360" activeTab="1" xr2:uid="{A535ECC4-06C6-4676-8CE5-90DAE0234A8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -161,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -185,7 +186,10 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -503,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD53D9B6-8549-4B30-B785-6BD17C328FBB}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +523,7 @@
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -529,17 +533,8 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>19</v>
       </c>
@@ -550,17 +545,8 @@
         <f>B2/B10</f>
         <v>0.125</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="9">
-        <v>18</v>
-      </c>
-      <c r="G2" s="9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>20</v>
       </c>
@@ -571,18 +557,8 @@
         <v>0.26</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="9">
-        <v>39</v>
-      </c>
-      <c r="G3" s="9">
-        <f t="shared" ref="G3:G8" si="0">F3-F2</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>21</v>
       </c>
@@ -593,18 +569,8 @@
         <f>(B4/B10)+C3</f>
         <v>0.39</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="9">
-        <v>64</v>
-      </c>
-      <c r="G4" s="9">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>22</v>
       </c>
@@ -614,18 +580,8 @@
       <c r="C5" s="7">
         <v>0.51</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="9">
-        <v>93</v>
-      </c>
-      <c r="G5" s="9">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>23</v>
       </c>
@@ -636,18 +592,8 @@
         <f>(B6/B10)+C5</f>
         <v>0.65500000000000003</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="9">
-        <v>115</v>
-      </c>
-      <c r="G6" s="9">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>24</v>
       </c>
@@ -657,18 +603,8 @@
       <c r="C7" s="7">
         <v>0.78500000000000003</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="9">
-        <v>132</v>
-      </c>
-      <c r="G7" s="9">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>25</v>
       </c>
@@ -679,47 +615,154 @@
         <f>(B8/B10)+C7</f>
         <v>0.9</v>
       </c>
-      <c r="E8" s="9" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>26</v>
+      </c>
+      <c r="B9" s="6">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
+        <v>200</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32018E5-CBE6-4B91-9BD9-B469A9D9CE2D}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10">
+        <v>18</v>
+      </c>
+      <c r="C2" s="10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="10">
+        <v>39</v>
+      </c>
+      <c r="C3" s="10">
+        <f t="shared" ref="C3:C8" si="0">B3-B2</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10">
+        <v>64</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="10">
+        <v>93</v>
+      </c>
+      <c r="C5" s="10">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="10">
+        <v>115</v>
+      </c>
+      <c r="C6" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
+        <v>132</v>
+      </c>
+      <c r="C7" s="10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="9">
+      <c r="B8" s="10">
         <v>140</v>
       </c>
-      <c r="G8" s="9">
+      <c r="C8" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>26</v>
-      </c>
-      <c r="B9" s="6">
-        <v>20</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="6">
-        <f>SUM(G2:G8)</f>
+      <c r="C9" s="9">
+        <f>SUM(C2:C8)</f>
         <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2">
-        <v>200</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>